<commit_message>
testando ajustes de nomes na geração da tabela
</commit_message>
<xml_diff>
--- a/TRIAGEM/pre-triagem-2021.xlsx
+++ b/TRIAGEM/pre-triagem-2021.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -497,28 +501,30 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>236813</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>236690</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Estudo Team.docx</t>
+          <t>Novas barreiras e tendências no comércio internacional.docx</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D2" t="n">
-        <v>131904</v>
+        <v>80889</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G2" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -526,43 +532,43 @@
       <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>01/02/2021</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>02/02/2021</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr"/>
+      <c r="J2" s="2" t="n">
+        <v>44221</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>236690</t>
+          <t>236813</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Novas barreiras e tendências no comércio internacional.docx</t>
+          <t>Estudo Team.docx</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D3" t="n">
-        <v>80889</v>
+        <v>131904</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G3" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -570,15 +576,11 @@
       <c r="I3" t="n">
         <v>0</v>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>25/01/2021</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>02/02/2021</t>
-        </is>
+      <c r="J3" s="2" t="n">
+        <v>44228</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>44229</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -592,18 +594,22 @@
           <t>233867</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>TESTE.docx</t>
+        </is>
+      </c>
       <c r="C4" t="n">
         <v>31</v>
       </c>
       <c r="D4" t="n">
-        <v>58108</v>
+        <v>56596</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="G4" t="n">
         <v>17</v>
@@ -614,15 +620,11 @@
       <c r="I4" t="n">
         <v>1</v>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>06/12/2019</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>02/02/2021</t>
-        </is>
+      <c r="J4" s="2" t="n">
+        <v>43805</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>44229</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>

</xml_diff>